<commit_message>
Exe 10 - Function
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/4.xay-dung-function.xlsx
+++ b/me/1.Lap-trinh-python/4.xay-dung-function.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89F7257C-B27C-6242-976A-ACD6FC962630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21DA9C25-7CFE-D743-8020-97F8891EB7EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="1660" windowWidth="29360" windowHeight="17440" activeTab="1" xr2:uid="{579F4252-B551-D846-AAD4-EA5CA4DAF042}"/>
+    <workbookView xWindow="2460" yWindow="1660" windowWidth="29360" windowHeight="17440" activeTab="2" xr2:uid="{579F4252-B551-D846-AAD4-EA5CA4DAF042}"/>
   </bookViews>
   <sheets>
     <sheet name="Function 01" sheetId="1" r:id="rId1"/>
     <sheet name="Function 02" sheetId="2" r:id="rId2"/>
+    <sheet name="Exe 10 - Function" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="106">
   <si>
     <t>構成</t>
   </si>
@@ -258,6 +259,102 @@
   </si>
   <si>
     <t>python3 02_return.py</t>
+  </si>
+  <si>
+    <t>exe_10_func.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_10_func.py</t>
+  </si>
+  <si>
+    <t># Input     : Cho 1 list chứa các khóa học</t>
+  </si>
+  <si>
+    <t># Output    : In ra thông tin khóa học</t>
+  </si>
+  <si>
+    <t># ---------Info - Start---------</t>
+  </si>
+  <si>
+    <t># -Name: PHP</t>
+  </si>
+  <si>
+    <t># -Type: Free</t>
+  </si>
+  <si>
+    <t># ==========Info - End==========</t>
+  </si>
+  <si>
+    <t>myList = [</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {'name': 'PHP', 'free': True},</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    {'name': 'Python', 'free': False}</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>def showCourseType(type):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if(type == True):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return "Free"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    else:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        return "No Free"</t>
+  </si>
+  <si>
+    <t>def showOutline(content, character = "-", newLine = False):</t>
+  </si>
+  <si>
+    <t>def showCourseInfo(course):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print("-Name: {name} \n-Type: {type}".format(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        name    = course['name'],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        type    = showCourseType(course['free']),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ))</t>
+  </si>
+  <si>
+    <t>def showList(myList):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for course in myList:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        showOutline("Info - Start")</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        showCourseInfo(course)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        showOutline("Info - End", "=", True)</t>
+  </si>
+  <si>
+    <t>showList(myList)</t>
+  </si>
+  <si>
+    <t>python3 exe_10_func.py</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    if (newLine == True): print (content.center(30, character), '\n')</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    else: print (content.center(30, character))</t>
   </si>
 </sst>
 </file>
@@ -407,8 +504,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,6 +886,55 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>203199</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>39856</xdr:colOff>
+      <xdr:row>95</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF9B2A90-5E52-5964-4CB4-41C891CFD782}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028699" y="16586200"/>
+          <a:ext cx="11393657" cy="2832100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -1565,8 +1711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9151EF5F-4D3A-7B49-A51F-9D3CF1E1FAE2}">
   <dimension ref="A3:P69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="J55" sqref="J55"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1722,7 +1868,7 @@
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="4"/>
-      <c r="D24" s="14" t="s">
+      <c r="D24" t="s">
         <v>34</v>
       </c>
       <c r="F24" s="5"/>
@@ -1841,140 +1987,92 @@
       <c r="B42" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="13"/>
-      <c r="D42" s="13"/>
-      <c r="E42" s="13"/>
       <c r="F42" s="5"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B43" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="13"/>
-      <c r="D43" s="13"/>
-      <c r="E43" s="13"/>
       <c r="F43" s="5"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B44" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C44" s="13"/>
-      <c r="D44" s="13"/>
-      <c r="E44" s="13"/>
       <c r="F44" s="5"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B45" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C45" s="13"/>
-      <c r="D45" s="13"/>
-      <c r="E45" s="13"/>
       <c r="F45" s="5"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B46" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="C46" s="13"/>
-      <c r="D46" s="13"/>
-      <c r="E46" s="13"/>
       <c r="F46" s="5"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B47" s="4"/>
-      <c r="C47" s="13"/>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
       <c r="F47" s="5"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B48" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="C48" s="13"/>
-      <c r="D48" s="13"/>
-      <c r="E48" s="13"/>
       <c r="F48" s="5"/>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B49" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C49" s="13"/>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
       <c r="F49" s="5"/>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B50" s="4"/>
-      <c r="C50" s="13"/>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
       <c r="F50" s="5"/>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B51" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="C51" s="13"/>
-      <c r="D51" s="13"/>
-      <c r="E51" s="13"/>
       <c r="F51" s="5"/>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B52" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C52" s="13"/>
-      <c r="D52" s="13"/>
-      <c r="E52" s="13"/>
       <c r="F52" s="5"/>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B53" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="C53" s="13"/>
-      <c r="D53" s="13"/>
-      <c r="E53" s="13"/>
       <c r="F53" s="5"/>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B54" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="C54" s="13"/>
-      <c r="D54" s="13"/>
-      <c r="E54" s="13"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B55" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C55" s="13"/>
-      <c r="D55" s="13"/>
-      <c r="E55" s="13"/>
       <c r="F55" s="5"/>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B56" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="13"/>
-      <c r="D56" s="13"/>
-      <c r="E56" s="13"/>
       <c r="F56" s="5"/>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B57" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C57" s="13"/>
-      <c r="D57" s="13"/>
-      <c r="E57" s="13"/>
       <c r="F57" s="5"/>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.2">
@@ -2006,130 +2104,33 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A62" s="4"/>
-      <c r="B62" s="13" t="s">
+      <c r="B62" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="13"/>
-      <c r="D62" s="13"/>
-      <c r="E62" s="13"/>
-      <c r="F62" s="13"/>
-      <c r="G62" s="13"/>
-      <c r="H62" s="13"/>
-      <c r="I62" s="13"/>
-      <c r="J62" s="13"/>
-      <c r="K62" s="13"/>
-      <c r="L62" s="13"/>
-      <c r="M62" s="13"/>
-      <c r="N62" s="13"/>
-      <c r="O62" s="13"/>
       <c r="P62" s="5"/>
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A63" s="4"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="13"/>
-      <c r="D63" s="13"/>
-      <c r="E63" s="13"/>
-      <c r="F63" s="13"/>
-      <c r="G63" s="13"/>
-      <c r="H63" s="13"/>
-      <c r="I63" s="13"/>
-      <c r="J63" s="13"/>
-      <c r="K63" s="13"/>
-      <c r="L63" s="13"/>
-      <c r="M63" s="13"/>
-      <c r="N63" s="13"/>
-      <c r="O63" s="13"/>
       <c r="P63" s="5"/>
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A64" s="4"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="13"/>
-      <c r="D64" s="13"/>
-      <c r="E64" s="13"/>
-      <c r="F64" s="13"/>
-      <c r="G64" s="13"/>
-      <c r="H64" s="13"/>
-      <c r="I64" s="13"/>
-      <c r="J64" s="13"/>
-      <c r="K64" s="13"/>
-      <c r="L64" s="13"/>
-      <c r="M64" s="13"/>
-      <c r="N64" s="13"/>
-      <c r="O64" s="13"/>
       <c r="P64" s="5"/>
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A65" s="4"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="13"/>
-      <c r="D65" s="13"/>
-      <c r="E65" s="13"/>
-      <c r="F65" s="13"/>
-      <c r="G65" s="13"/>
-      <c r="H65" s="13"/>
-      <c r="I65" s="13"/>
-      <c r="J65" s="13"/>
-      <c r="K65" s="13"/>
-      <c r="L65" s="13"/>
-      <c r="M65" s="13"/>
-      <c r="N65" s="13"/>
-      <c r="O65" s="13"/>
       <c r="P65" s="5"/>
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A66" s="4"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="13"/>
-      <c r="D66" s="13"/>
-      <c r="E66" s="13"/>
-      <c r="F66" s="13"/>
-      <c r="G66" s="13"/>
-      <c r="H66" s="13"/>
-      <c r="I66" s="13"/>
-      <c r="J66" s="13"/>
-      <c r="K66" s="13"/>
-      <c r="L66" s="13"/>
-      <c r="M66" s="13"/>
-      <c r="N66" s="13"/>
-      <c r="O66" s="13"/>
       <c r="P66" s="5"/>
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A67" s="4"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="13"/>
-      <c r="D67" s="13"/>
-      <c r="E67" s="13"/>
-      <c r="F67" s="13"/>
-      <c r="G67" s="13"/>
-      <c r="H67" s="13"/>
-      <c r="I67" s="13"/>
-      <c r="J67" s="13"/>
-      <c r="K67" s="13"/>
-      <c r="L67" s="13"/>
-      <c r="M67" s="13"/>
-      <c r="N67" s="13"/>
-      <c r="O67" s="13"/>
       <c r="P67" s="5"/>
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A68" s="4"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="13"/>
-      <c r="D68" s="13"/>
-      <c r="E68" s="13"/>
-      <c r="F68" s="13"/>
-      <c r="G68" s="13"/>
-      <c r="H68" s="13"/>
-      <c r="I68" s="13"/>
-      <c r="J68" s="13"/>
-      <c r="K68" s="13"/>
-      <c r="L68" s="13"/>
-      <c r="M68" s="13"/>
-      <c r="N68" s="13"/>
-      <c r="O68" s="13"/>
       <c r="P68" s="5"/>
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.2">
@@ -2154,4 +2155,940 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1C199E-6803-584E-BDA3-1B7CD5B5548B}">
+  <dimension ref="A3:P96"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="P107" sqref="P107"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="4"/>
+      <c r="C5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="4"/>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="4"/>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="4"/>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="4"/>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="5"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="4"/>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="4"/>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="4"/>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="5"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="4"/>
+      <c r="D14" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="5"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="4"/>
+      <c r="D15" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="4"/>
+      <c r="D16" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="4"/>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="5"/>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="4"/>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="7"/>
+      <c r="F18" s="5"/>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="4"/>
+      <c r="D19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="5"/>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="4"/>
+      <c r="D20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" s="5"/>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="4"/>
+      <c r="D21" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="5"/>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="4"/>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="4"/>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="4"/>
+      <c r="D24" t="s">
+        <v>34</v>
+      </c>
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="4"/>
+      <c r="D25" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F25" s="5"/>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="5"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="4"/>
+      <c r="C27" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="5"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="4"/>
+      <c r="C28" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="5"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="4"/>
+      <c r="C29" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="5"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="4"/>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="5"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="4"/>
+      <c r="C31" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="5"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="4"/>
+      <c r="C32" t="s">
+        <v>26</v>
+      </c>
+      <c r="F32" s="5"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="4"/>
+      <c r="C33" t="s">
+        <v>27</v>
+      </c>
+      <c r="F33" s="5"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B34" s="4"/>
+      <c r="C34" t="s">
+        <v>28</v>
+      </c>
+      <c r="F34" s="5"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="4"/>
+      <c r="C35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="5"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="4"/>
+      <c r="C36" t="s">
+        <v>30</v>
+      </c>
+      <c r="F36" s="5"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="4"/>
+      <c r="C37" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" t="s">
+        <v>31</v>
+      </c>
+      <c r="H37" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="8"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="9"/>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="3"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B43" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" s="14"/>
+      <c r="D43" s="14"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="14"/>
+      <c r="G43" s="5"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B44" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="14"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="14"/>
+      <c r="G44" s="5"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B45" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C45" s="14"/>
+      <c r="D45" s="14"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="14"/>
+      <c r="G45" s="5"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B46" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" s="14"/>
+      <c r="D46" s="14"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="14"/>
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B47" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="C47" s="14"/>
+      <c r="D47" s="14"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="14"/>
+      <c r="G47" s="5"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B48" s="4"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="5"/>
+    </row>
+    <row r="49" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B49" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" s="14"/>
+      <c r="D49" s="14"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="14"/>
+      <c r="G49" s="5"/>
+    </row>
+    <row r="50" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B50" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C50" s="14"/>
+      <c r="D50" s="14"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="14"/>
+      <c r="G50" s="5"/>
+    </row>
+    <row r="51" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B51" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C51" s="14"/>
+      <c r="D51" s="14"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="14"/>
+      <c r="G51" s="5"/>
+    </row>
+    <row r="52" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B52" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C52" s="14"/>
+      <c r="D52" s="14"/>
+      <c r="E52" s="14"/>
+      <c r="F52" s="14"/>
+      <c r="G52" s="5"/>
+    </row>
+    <row r="53" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B53" s="4"/>
+      <c r="C53" s="14"/>
+      <c r="D53" s="14"/>
+      <c r="E53" s="14"/>
+      <c r="F53" s="14"/>
+      <c r="G53" s="5"/>
+    </row>
+    <row r="54" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B54" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C54" s="14"/>
+      <c r="D54" s="14"/>
+      <c r="E54" s="14"/>
+      <c r="F54" s="14"/>
+      <c r="G54" s="5"/>
+    </row>
+    <row r="55" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B55" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C55" s="14"/>
+      <c r="D55" s="14"/>
+      <c r="E55" s="14"/>
+      <c r="F55" s="14"/>
+      <c r="G55" s="5"/>
+    </row>
+    <row r="56" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B56" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C56" s="14"/>
+      <c r="D56" s="14"/>
+      <c r="E56" s="14"/>
+      <c r="F56" s="14"/>
+      <c r="G56" s="5"/>
+    </row>
+    <row r="57" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B57" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C57" s="14"/>
+      <c r="D57" s="14"/>
+      <c r="E57" s="14"/>
+      <c r="F57" s="14"/>
+      <c r="G57" s="5"/>
+    </row>
+    <row r="58" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B58" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C58" s="14"/>
+      <c r="D58" s="14"/>
+      <c r="E58" s="14"/>
+      <c r="F58" s="14"/>
+      <c r="G58" s="5"/>
+    </row>
+    <row r="59" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B59" s="4"/>
+      <c r="C59" s="14"/>
+      <c r="D59" s="14"/>
+      <c r="E59" s="14"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="5"/>
+    </row>
+    <row r="60" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B60" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C60" s="14"/>
+      <c r="D60" s="14"/>
+      <c r="E60" s="14"/>
+      <c r="F60" s="14"/>
+      <c r="G60" s="5"/>
+    </row>
+    <row r="61" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B61" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C61" s="14"/>
+      <c r="D61" s="14"/>
+      <c r="E61" s="14"/>
+      <c r="F61" s="14"/>
+      <c r="G61" s="5"/>
+    </row>
+    <row r="62" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B62" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C62" s="14"/>
+      <c r="D62" s="14"/>
+      <c r="E62" s="14"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="5"/>
+    </row>
+    <row r="63" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B63" s="4"/>
+      <c r="C63" s="14"/>
+      <c r="D63" s="14"/>
+      <c r="E63" s="14"/>
+      <c r="F63" s="14"/>
+      <c r="G63" s="5"/>
+    </row>
+    <row r="64" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B64" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="14"/>
+      <c r="E64" s="14"/>
+      <c r="F64" s="14"/>
+      <c r="G64" s="5"/>
+    </row>
+    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B65" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" s="14"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="5"/>
+    </row>
+    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B66" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="14"/>
+      <c r="D66" s="14"/>
+      <c r="E66" s="14"/>
+      <c r="F66" s="14"/>
+      <c r="G66" s="5"/>
+    </row>
+    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B67" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C67" s="14"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="14"/>
+      <c r="F67" s="14"/>
+      <c r="G67" s="5"/>
+    </row>
+    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B68" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C68" s="14"/>
+      <c r="D68" s="14"/>
+      <c r="E68" s="14"/>
+      <c r="F68" s="14"/>
+      <c r="G68" s="5"/>
+    </row>
+    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B69" s="4"/>
+      <c r="C69" s="14"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="14"/>
+      <c r="F69" s="14"/>
+      <c r="G69" s="5"/>
+    </row>
+    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B70" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C70" s="14"/>
+      <c r="D70" s="14"/>
+      <c r="E70" s="14"/>
+      <c r="F70" s="14"/>
+      <c r="G70" s="5"/>
+    </row>
+    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B71" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="14"/>
+      <c r="E71" s="14"/>
+      <c r="F71" s="14"/>
+      <c r="G71" s="5"/>
+    </row>
+    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B72" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C72" s="14"/>
+      <c r="D72" s="14"/>
+      <c r="E72" s="14"/>
+      <c r="F72" s="14"/>
+      <c r="G72" s="5"/>
+    </row>
+    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B73" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="5"/>
+    </row>
+    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B74" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C74" s="14"/>
+      <c r="D74" s="14"/>
+      <c r="E74" s="14"/>
+      <c r="F74" s="14"/>
+      <c r="G74" s="5"/>
+    </row>
+    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B75" s="4"/>
+      <c r="C75" s="14"/>
+      <c r="D75" s="14"/>
+      <c r="E75" s="14"/>
+      <c r="F75" s="14"/>
+      <c r="G75" s="5"/>
+    </row>
+    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B76" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C76" s="14"/>
+      <c r="D76" s="14"/>
+      <c r="E76" s="14"/>
+      <c r="F76" s="14"/>
+      <c r="G76" s="5"/>
+    </row>
+    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="B77" s="8"/>
+      <c r="C77" s="9"/>
+      <c r="D77" s="9"/>
+      <c r="E77" s="9"/>
+      <c r="F77" s="9"/>
+      <c r="G77" s="10"/>
+    </row>
+    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A80" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B80" s="2"/>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+      <c r="E80" s="2"/>
+      <c r="F80" s="2"/>
+      <c r="G80" s="2"/>
+      <c r="H80" s="2"/>
+      <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
+      <c r="L80" s="2"/>
+      <c r="M80" s="2"/>
+      <c r="N80" s="2"/>
+      <c r="O80" s="2"/>
+      <c r="P80" s="3"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+      <c r="B81" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C81" s="14"/>
+      <c r="D81" s="14"/>
+      <c r="E81" s="14"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="14"/>
+      <c r="H81" s="14"/>
+      <c r="I81" s="14"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
+      <c r="N81" s="14"/>
+      <c r="O81" s="14"/>
+      <c r="P81" s="5"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A82" s="4"/>
+      <c r="B82" s="14"/>
+      <c r="C82" s="14"/>
+      <c r="D82" s="14"/>
+      <c r="E82" s="14"/>
+      <c r="F82" s="14"/>
+      <c r="G82" s="14"/>
+      <c r="H82" s="14"/>
+      <c r="I82" s="14"/>
+      <c r="J82" s="14"/>
+      <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
+      <c r="N82" s="14"/>
+      <c r="O82" s="14"/>
+      <c r="P82" s="5"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A83" s="4"/>
+      <c r="B83" s="14"/>
+      <c r="C83" s="14"/>
+      <c r="D83" s="14"/>
+      <c r="E83" s="14"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="14"/>
+      <c r="H83" s="14"/>
+      <c r="I83" s="14"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
+      <c r="N83" s="14"/>
+      <c r="O83" s="14"/>
+      <c r="P83" s="5"/>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A84" s="4"/>
+      <c r="B84" s="14"/>
+      <c r="C84" s="14"/>
+      <c r="D84" s="14"/>
+      <c r="E84" s="14"/>
+      <c r="F84" s="14"/>
+      <c r="G84" s="14"/>
+      <c r="H84" s="14"/>
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
+      <c r="N84" s="14"/>
+      <c r="O84" s="14"/>
+      <c r="P84" s="5"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A85" s="4"/>
+      <c r="B85" s="14"/>
+      <c r="C85" s="14"/>
+      <c r="D85" s="14"/>
+      <c r="E85" s="14"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="14"/>
+      <c r="H85" s="14"/>
+      <c r="I85" s="14"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="14"/>
+      <c r="L85" s="14"/>
+      <c r="M85" s="14"/>
+      <c r="N85" s="14"/>
+      <c r="O85" s="14"/>
+      <c r="P85" s="5"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A86" s="4"/>
+      <c r="B86" s="14"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="14"/>
+      <c r="J86" s="14"/>
+      <c r="K86" s="14"/>
+      <c r="L86" s="14"/>
+      <c r="M86" s="14"/>
+      <c r="N86" s="14"/>
+      <c r="O86" s="14"/>
+      <c r="P86" s="5"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A87" s="4"/>
+      <c r="B87" s="14"/>
+      <c r="C87" s="14"/>
+      <c r="D87" s="14"/>
+      <c r="E87" s="14"/>
+      <c r="F87" s="14"/>
+      <c r="G87" s="14"/>
+      <c r="H87" s="14"/>
+      <c r="I87" s="14"/>
+      <c r="J87" s="14"/>
+      <c r="K87" s="14"/>
+      <c r="L87" s="14"/>
+      <c r="M87" s="14"/>
+      <c r="N87" s="14"/>
+      <c r="O87" s="14"/>
+      <c r="P87" s="5"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A88" s="4"/>
+      <c r="B88" s="14"/>
+      <c r="C88" s="14"/>
+      <c r="D88" s="14"/>
+      <c r="E88" s="14"/>
+      <c r="F88" s="14"/>
+      <c r="G88" s="14"/>
+      <c r="H88" s="14"/>
+      <c r="I88" s="14"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
+      <c r="M88" s="14"/>
+      <c r="N88" s="14"/>
+      <c r="O88" s="14"/>
+      <c r="P88" s="5"/>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A89" s="4"/>
+      <c r="B89" s="14"/>
+      <c r="C89" s="14"/>
+      <c r="D89" s="14"/>
+      <c r="E89" s="14"/>
+      <c r="F89" s="14"/>
+      <c r="G89" s="14"/>
+      <c r="H89" s="14"/>
+      <c r="I89" s="14"/>
+      <c r="J89" s="14"/>
+      <c r="K89" s="14"/>
+      <c r="L89" s="14"/>
+      <c r="M89" s="14"/>
+      <c r="N89" s="14"/>
+      <c r="O89" s="14"/>
+      <c r="P89" s="5"/>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A90" s="4"/>
+      <c r="B90" s="14"/>
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="14"/>
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+      <c r="H90" s="14"/>
+      <c r="I90" s="14"/>
+      <c r="J90" s="14"/>
+      <c r="K90" s="14"/>
+      <c r="L90" s="14"/>
+      <c r="M90" s="14"/>
+      <c r="N90" s="14"/>
+      <c r="O90" s="14"/>
+      <c r="P90" s="5"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A91" s="4"/>
+      <c r="B91" s="14"/>
+      <c r="C91" s="14"/>
+      <c r="D91" s="14"/>
+      <c r="E91" s="14"/>
+      <c r="F91" s="14"/>
+      <c r="G91" s="14"/>
+      <c r="H91" s="14"/>
+      <c r="I91" s="14"/>
+      <c r="J91" s="14"/>
+      <c r="K91" s="14"/>
+      <c r="L91" s="14"/>
+      <c r="M91" s="14"/>
+      <c r="N91" s="14"/>
+      <c r="O91" s="14"/>
+      <c r="P91" s="5"/>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A92" s="4"/>
+      <c r="B92" s="14"/>
+      <c r="C92" s="14"/>
+      <c r="D92" s="14"/>
+      <c r="E92" s="14"/>
+      <c r="F92" s="14"/>
+      <c r="G92" s="14"/>
+      <c r="H92" s="14"/>
+      <c r="I92" s="14"/>
+      <c r="J92" s="14"/>
+      <c r="K92" s="14"/>
+      <c r="L92" s="14"/>
+      <c r="M92" s="14"/>
+      <c r="N92" s="14"/>
+      <c r="O92" s="14"/>
+      <c r="P92" s="5"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A93" s="4"/>
+      <c r="B93" s="14"/>
+      <c r="C93" s="14"/>
+      <c r="D93" s="14"/>
+      <c r="E93" s="14"/>
+      <c r="F93" s="14"/>
+      <c r="G93" s="14"/>
+      <c r="H93" s="14"/>
+      <c r="I93" s="14"/>
+      <c r="J93" s="14"/>
+      <c r="K93" s="14"/>
+      <c r="L93" s="14"/>
+      <c r="M93" s="14"/>
+      <c r="N93" s="14"/>
+      <c r="O93" s="14"/>
+      <c r="P93" s="5"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A94" s="4"/>
+      <c r="B94" s="14"/>
+      <c r="C94" s="14"/>
+      <c r="D94" s="14"/>
+      <c r="E94" s="14"/>
+      <c r="F94" s="14"/>
+      <c r="G94" s="14"/>
+      <c r="H94" s="14"/>
+      <c r="I94" s="14"/>
+      <c r="J94" s="14"/>
+      <c r="K94" s="14"/>
+      <c r="L94" s="14"/>
+      <c r="M94" s="14"/>
+      <c r="N94" s="14"/>
+      <c r="O94" s="14"/>
+      <c r="P94" s="5"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A95" s="4"/>
+      <c r="B95" s="14"/>
+      <c r="C95" s="14"/>
+      <c r="D95" s="14"/>
+      <c r="E95" s="14"/>
+      <c r="F95" s="14"/>
+      <c r="G95" s="14"/>
+      <c r="H95" s="14"/>
+      <c r="I95" s="14"/>
+      <c r="J95" s="14"/>
+      <c r="K95" s="14"/>
+      <c r="L95" s="14"/>
+      <c r="M95" s="14"/>
+      <c r="N95" s="14"/>
+      <c r="O95" s="14"/>
+      <c r="P95" s="5"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="9"/>
+      <c r="G96" s="9"/>
+      <c r="H96" s="9"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="9"/>
+      <c r="K96" s="9"/>
+      <c r="L96" s="9"/>
+      <c r="M96" s="9"/>
+      <c r="N96" s="9"/>
+      <c r="O96" s="9"/>
+      <c r="P96" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>